<commit_message>
No conformidades de proyecto
</commit_message>
<xml_diff>
--- a/Proyectos/2015/11/P1339 - DA3 - CBANT, Héctor Antonio Núñez Ruiz_OC/Calidad/No_conformidades_P1339.xlsx
+++ b/Proyectos/2015/11/P1339 - DA3 - CBANT, Héctor Antonio Núñez Ruiz_OC/Calidad/No_conformidades_P1339.xlsx
@@ -17,10 +17,8 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
-    <r>
-      <t>REPORTE DE NO CONFORMIDADES P1339 - DA3 - CBANT, Héctor Antonio Núñez Ruiz_OC
+    <t>REPORTE DE NO CONFORMIDADES P1339 - DA3 - CBANT, Héctor Antonio Núñez Ruiz_OC
 </t>
-    </r>
   </si>
   <si>
     <t>ID</t>
@@ -103,7 +101,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -135,12 +133,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -154,12 +146,6 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -236,7 +222,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -245,7 +231,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -265,12 +251,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -352,8 +334,8 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -475,7 +457,7 @@
         <v>42353</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>16</v>
@@ -498,7 +480,7 @@
         <v>42353</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>18</v>
@@ -520,8 +502,8 @@
       <c r="E8" s="5" t="n">
         <v>42353</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>13</v>
+      <c r="F8" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>20</v>
@@ -543,8 +525,8 @@
       <c r="E9" s="5" t="n">
         <v>42353</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>13</v>
+      <c r="F9" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>22</v>

</xml_diff>